<commit_message>
add: Se agrega acuse de vales grandeza
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteNominaValesv3.xlsx
+++ b/public/archivos/formatoReporteNominaValesv3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nugasoft/react/vales/apivales/public/archivos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB21808-0B65-D649-AC24-4CE2DE282B40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8939B86A-BF77-FA4E-904B-12045763A4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="6100" windowWidth="46580" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
@@ -303,23 +303,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>54429</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>92321</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>435427</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>217713</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2345472</xdr:colOff>
+      <xdr:colOff>72570</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>272144</xdr:rowOff>
+      <xdr:rowOff>228599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Imagen 11">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90407E57-2B6F-4FD0-80B4-A30F270570F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0576C21-D12C-487E-FD66-836235D61F3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -335,18 +335,20 @@
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="707572" y="1017607"/>
-          <a:ext cx="7516186" cy="1105108"/>
+          <a:off x="435427" y="217713"/>
+          <a:ext cx="5515429" cy="1861457"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>

</xml_diff>

<commit_message>
Update: Cambios en módulo de entrega de vales
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteNominaValesv3.xlsx
+++ b/public/archivos/formatoReporteNominaValesv3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D45F19-5B62-CE45-9377-DA1C5B657519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E5230-97C9-ED4D-92B2-B0A04C736CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
@@ -228,20 +228,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +586,7 @@
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,34 +622,34 @@
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:27" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:27" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:27" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
@@ -659,10 +659,10 @@
       <c r="E4" s="10"/>
       <c r="F4" s="9"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
     </row>
@@ -673,7 +673,7 @@
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="16"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="10"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
@@ -688,7 +688,7 @@
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
@@ -703,7 +703,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="14"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>

</xml_diff>